<commit_message>
correction html et godmod
</commit_message>
<xml_diff>
--- a/Quete/Taverne4.xlsx
+++ b/Quete/Taverne4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D434BE-06EE-41B4-9823-FFAAC926D1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D50D19-78E8-4EF1-8214-1F6CE550A6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Chap</t>
   </si>
@@ -111,6 +111,61 @@
   </si>
   <si>
     <t>output_test_4</t>
+  </si>
+  <si>
+    <t>Les n nombres</t>
+  </si>
+  <si>
+    <t>Ecrivez un programme qui crée une liste vide nommée L et qui ajoute ensuite à cette liste n nombres entiers, compris entre 1 et 10, saisis par l'utilisateur. 
+Finalement, le programme affichera toute la liste ainsi que chaque élément de la liste séparément</t>
+  </si>
+  <si>
+    <t>5
+1
+2
+3
+4
+5</t>
+  </si>
+  <si>
+    <t>2
+6
+9</t>
+  </si>
+  <si>
+    <t>8
+4
+4
+4
+4
+6
+6
+4
+5</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 4, 5]
+L[0] = 1
+L[1] = 2
+L[2] = 3
+L[3] = 4
+L[4] = 5</t>
+  </si>
+  <si>
+    <t>[6, 9]
+L[0] = 6
+L[1] = 9</t>
+  </si>
+  <si>
+    <t>[4, 4, 4, 4, 6, 6, 4, 5]
+L[0] = 4
+L[1] = 4
+L[2] = 4
+L[3] = 4
+L[4] = 6
+L[5] = 6
+L[6] = 4
+L[7] = 5</t>
   </si>
 </sst>
 </file>
@@ -496,12 +551,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" customWidth="1"/>
     <col min="7" max="7" width="20.5546875" customWidth="1"/>
@@ -589,29 +645,65 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
+      <c r="Q2" s="1">
+        <v>3</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>

</xml_diff>